<commit_message>
DM EZ Themes first draft
</commit_message>
<xml_diff>
--- a/DataInput/Updated_Yan-Zheng-Compustat-Vars.xlsx
+++ b/DataInput/Updated_Yan-Zheng-Compustat-Vars.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Risk-vs-ac\flex-mining\DataInput\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20B8FFC-C1F5-45FD-B844-0582028E367D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2145" yWindow="-120" windowWidth="26775" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="636">
   <si>
     <t>id</t>
   </si>
@@ -1513,9 +1519,6 @@
     <t xml:space="preserve">Assets </t>
   </si>
   <si>
-    <t>Cap surplus reserve</t>
-  </si>
-  <si>
     <t>Capex PPE sch V</t>
   </si>
   <si>
@@ -1546,9 +1549,6 @@
     <t>Common stock</t>
   </si>
   <si>
-    <t>Common stock equivalents dollar savings</t>
-  </si>
-  <si>
     <t>Debt convertible</t>
   </si>
   <si>
@@ -1651,12 +1651,6 @@
     <t>Income bef extraord</t>
   </si>
   <si>
-    <t>Income before extraordinary items cf</t>
-  </si>
-  <si>
-    <t>Income bf extraordinary</t>
-  </si>
-  <si>
     <t xml:space="preserve">Invested capital </t>
   </si>
   <si>
@@ -1913,13 +1907,34 @@
   </si>
   <si>
     <t>Market equity FYE</t>
+  </si>
+  <si>
+    <t>Merger income contrib</t>
+  </si>
+  <si>
+    <t>Merger sales contrib</t>
+  </si>
+  <si>
+    <t>Capital surplus</t>
+  </si>
+  <si>
+    <t>Common stock equivalents</t>
+  </si>
+  <si>
+    <t>LitCat</t>
+  </si>
+  <si>
+    <t>Income bef extraord cf</t>
+  </si>
+  <si>
+    <t>Income bef extraord common</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1944,7 +1959,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1967,13 +1982,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1982,13 +2011,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2026,7 +2063,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2060,6 +2097,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2094,9 +2132,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2269,14 +2308,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G243"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2298,8 +2348,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2319,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2339,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2359,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2379,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2399,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2419,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2439,7 +2492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2459,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2479,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2499,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2519,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2530,7 +2583,7 @@
         <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>629</v>
       </c>
       <c r="E13">
         <v>32</v>
@@ -2539,7 +2592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2550,7 +2603,7 @@
         <v>261</v>
       </c>
       <c r="D14" t="s">
-        <v>261</v>
+        <v>630</v>
       </c>
       <c r="E14">
         <v>31</v>
@@ -2559,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2579,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2599,7 +2652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2610,7 +2663,7 @@
         <v>264</v>
       </c>
       <c r="D17" t="s">
-        <v>499</v>
+        <v>631</v>
       </c>
       <c r="E17">
         <v>19</v>
@@ -2619,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2639,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2650,7 +2703,7 @@
         <v>266</v>
       </c>
       <c r="D19" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E19">
         <v>15</v>
@@ -2659,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2670,7 +2723,7 @@
         <v>267</v>
       </c>
       <c r="D20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E20">
         <v>13</v>
@@ -2679,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2690,7 +2743,7 @@
         <v>268</v>
       </c>
       <c r="D21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E21">
         <v>16</v>
@@ -2699,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2719,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2739,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2750,7 +2803,7 @@
         <v>271</v>
       </c>
       <c r="D24" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E24">
         <v>21</v>
@@ -2759,7 +2812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2770,7 +2823,7 @@
         <v>272</v>
       </c>
       <c r="D25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E25">
         <v>32</v>
@@ -2779,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2790,7 +2843,7 @@
         <v>273</v>
       </c>
       <c r="D26" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E26">
         <v>34</v>
@@ -2799,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2810,7 +2863,7 @@
         <v>274</v>
       </c>
       <c r="D27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E27">
         <v>34</v>
@@ -2819,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2830,7 +2883,7 @@
         <v>275</v>
       </c>
       <c r="D28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E28">
         <v>34</v>
@@ -2839,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2850,7 +2903,7 @@
         <v>276</v>
       </c>
       <c r="D29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E29">
         <v>34</v>
@@ -2859,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2879,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2890,7 +2943,7 @@
         <v>278</v>
       </c>
       <c r="D31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E31">
         <v>12</v>
@@ -2899,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2919,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2930,7 +2983,7 @@
         <v>280</v>
       </c>
       <c r="D33" t="s">
-        <v>510</v>
+        <v>632</v>
       </c>
       <c r="E33">
         <v>39</v>
@@ -2939,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2959,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2979,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2999,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3019,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3039,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3059,7 +3112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3070,7 +3123,7 @@
         <v>287</v>
       </c>
       <c r="D40" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E40">
         <v>16</v>
@@ -3079,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3099,7 +3152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3119,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3139,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3159,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3179,7 +3232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3199,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3219,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3239,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3259,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3279,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3290,7 +3343,7 @@
         <v>298</v>
       </c>
       <c r="D51" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E51">
         <v>20</v>
@@ -3299,7 +3352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3319,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3339,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3359,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3379,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3399,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3410,7 +3463,7 @@
         <v>304</v>
       </c>
       <c r="D57" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E57">
         <v>15</v>
@@ -3419,7 +3472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3439,7 +3492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3459,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3470,7 +3523,7 @@
         <v>307</v>
       </c>
       <c r="D60" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E60">
         <v>36</v>
@@ -3479,7 +3532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3499,7 +3552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3510,7 +3563,7 @@
         <v>309</v>
       </c>
       <c r="D62" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E62">
         <v>20</v>
@@ -3519,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3530,7 +3583,7 @@
         <v>310</v>
       </c>
       <c r="D63" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E63">
         <v>23</v>
@@ -3539,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3550,7 +3603,7 @@
         <v>311</v>
       </c>
       <c r="D64" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E64">
         <v>22</v>
@@ -3559,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3570,7 +3623,7 @@
         <v>312</v>
       </c>
       <c r="D65" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E65">
         <v>23</v>
@@ -3579,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3590,7 +3643,7 @@
         <v>313</v>
       </c>
       <c r="D66" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E66">
         <v>27</v>
@@ -3599,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3610,7 +3663,7 @@
         <v>314</v>
       </c>
       <c r="D67" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E67">
         <v>25</v>
@@ -3619,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3639,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3659,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3679,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3690,7 +3743,7 @@
         <v>318</v>
       </c>
       <c r="D71" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E71">
         <v>14</v>
@@ -3699,7 +3752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3710,7 +3763,7 @@
         <v>319</v>
       </c>
       <c r="D72" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E72">
         <v>16</v>
@@ -3719,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3730,7 +3783,7 @@
         <v>320</v>
       </c>
       <c r="D73" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E73">
         <v>14</v>
@@ -3739,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3759,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3770,7 +3823,7 @@
         <v>322</v>
       </c>
       <c r="D75" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E75">
         <v>20</v>
@@ -3779,7 +3832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3790,7 +3843,7 @@
         <v>323</v>
       </c>
       <c r="D76" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E76">
         <v>10</v>
@@ -3799,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3810,7 +3863,7 @@
         <v>324</v>
       </c>
       <c r="D77" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E77">
         <v>29</v>
@@ -3819,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3830,7 +3883,7 @@
         <v>325</v>
       </c>
       <c r="D78" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E78">
         <v>29</v>
@@ -3839,7 +3892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3850,7 +3903,7 @@
         <v>326</v>
       </c>
       <c r="D79" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E79">
         <v>29</v>
@@ -3859,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3870,7 +3923,7 @@
         <v>327</v>
       </c>
       <c r="D80" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E80">
         <v>29</v>
@@ -3879,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3899,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3919,7 +3972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3930,7 +3983,7 @@
         <v>330</v>
       </c>
       <c r="D83" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E83">
         <v>25</v>
@@ -3939,7 +3992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3950,7 +4003,7 @@
         <v>331</v>
       </c>
       <c r="D84" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E84">
         <v>19</v>
@@ -3959,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3970,7 +4023,7 @@
         <v>332</v>
       </c>
       <c r="D85" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E85">
         <v>26</v>
@@ -3979,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3990,7 +4043,7 @@
         <v>333</v>
       </c>
       <c r="D86" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E86">
         <v>46</v>
@@ -3999,7 +4052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4019,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4039,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4050,7 +4103,7 @@
         <v>336</v>
       </c>
       <c r="D89" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E89">
         <v>13</v>
@@ -4059,7 +4112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4070,7 +4123,7 @@
         <v>337</v>
       </c>
       <c r="D90" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E90">
         <v>28</v>
@@ -4079,7 +4132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4090,7 +4143,7 @@
         <v>338</v>
       </c>
       <c r="D91" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E91">
         <v>17</v>
@@ -4099,7 +4152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4110,7 +4163,7 @@
         <v>339</v>
       </c>
       <c r="D92" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E92">
         <v>10</v>
@@ -4119,7 +4172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4130,7 +4183,7 @@
         <v>340</v>
       </c>
       <c r="D93" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E93">
         <v>25</v>
@@ -4139,7 +4192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4150,7 +4203,7 @@
         <v>341</v>
       </c>
       <c r="D94" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E94">
         <v>9</v>
@@ -4159,7 +4212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4170,7 +4223,7 @@
         <v>342</v>
       </c>
       <c r="D95" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E95">
         <v>25</v>
@@ -4179,7 +4232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4199,7 +4252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4219,7 +4272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4239,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4250,7 +4303,7 @@
         <v>346</v>
       </c>
       <c r="D99" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E99">
         <v>51</v>
@@ -4259,7 +4312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4270,7 +4323,7 @@
         <v>347</v>
       </c>
       <c r="D100" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E100">
         <v>21</v>
@@ -4279,7 +4332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4299,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4319,7 +4372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4339,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4359,7 +4412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4379,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4390,7 +4443,7 @@
         <v>353</v>
       </c>
       <c r="D106" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E106">
         <v>13</v>
@@ -4399,7 +4452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4410,7 +4463,7 @@
         <v>354</v>
       </c>
       <c r="D107" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E107">
         <v>19</v>
@@ -4419,7 +4472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4439,7 +4492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4450,7 +4503,7 @@
         <v>356</v>
       </c>
       <c r="D109" t="s">
-        <v>545</v>
+        <v>634</v>
       </c>
       <c r="E109">
         <v>36</v>
@@ -4459,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4470,7 +4523,7 @@
         <v>357</v>
       </c>
       <c r="D110" t="s">
-        <v>546</v>
+        <v>635</v>
       </c>
       <c r="E110">
         <v>23</v>
@@ -4479,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4490,7 +4543,7 @@
         <v>358</v>
       </c>
       <c r="D111" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="E111">
         <v>17</v>
@@ -4499,7 +4552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4510,7 +4563,7 @@
         <v>359</v>
       </c>
       <c r="D112" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="E112">
         <v>28</v>
@@ -4519,7 +4572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4530,7 +4583,7 @@
         <v>360</v>
       </c>
       <c r="D113" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="E113">
         <v>18</v>
@@ -4539,7 +4592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4559,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4579,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4590,7 +4643,7 @@
         <v>363</v>
       </c>
       <c r="D116" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="E116">
         <v>18</v>
@@ -4599,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4619,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4639,7 +4692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4659,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4670,7 +4723,7 @@
         <v>367</v>
       </c>
       <c r="D120" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E120">
         <v>12</v>
@@ -4679,7 +4732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4699,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4710,7 +4763,7 @@
         <v>369</v>
       </c>
       <c r="D122" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="E122">
         <v>21</v>
@@ -4719,7 +4772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4730,7 +4783,7 @@
         <v>370</v>
       </c>
       <c r="D123" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="E123">
         <v>26</v>
@@ -4739,7 +4792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4759,7 +4812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4770,7 +4823,7 @@
         <v>372</v>
       </c>
       <c r="D125" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E125">
         <v>24</v>
@@ -4779,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4790,7 +4843,7 @@
         <v>373</v>
       </c>
       <c r="D126" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="E126">
         <v>23</v>
@@ -4799,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4819,7 +4872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4839,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4850,7 +4903,7 @@
         <v>376</v>
       </c>
       <c r="D129" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="E129">
         <v>23</v>
@@ -4859,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4870,7 +4923,7 @@
         <v>377</v>
       </c>
       <c r="D130" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="E130">
         <v>21</v>
@@ -4879,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4899,7 +4952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4919,7 +4972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4939,7 +4992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4950,7 +5003,7 @@
         <v>381</v>
       </c>
       <c r="D134" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E134">
         <v>20</v>
@@ -4959,7 +5012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4979,7 +5032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4990,7 +5043,7 @@
         <v>383</v>
       </c>
       <c r="D136" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="E136">
         <v>18</v>
@@ -4999,7 +5052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5010,7 +5063,7 @@
         <v>384</v>
       </c>
       <c r="D137" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="E137">
         <v>12</v>
@@ -5019,7 +5072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5030,7 +5083,7 @@
         <v>385</v>
       </c>
       <c r="D138" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="E138">
         <v>17</v>
@@ -5039,7 +5092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5059,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5070,7 +5123,7 @@
         <v>387</v>
       </c>
       <c r="D140" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="E140">
         <v>26</v>
@@ -5079,7 +5132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5090,7 +5143,7 @@
         <v>388</v>
       </c>
       <c r="D141" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E141">
         <v>26</v>
@@ -5099,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5110,7 +5163,7 @@
         <v>389</v>
       </c>
       <c r="D142" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="E142">
         <v>26</v>
@@ -5119,7 +5172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5130,7 +5183,7 @@
         <v>390</v>
       </c>
       <c r="D143" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="E143">
         <v>26</v>
@@ -5139,7 +5192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5150,7 +5203,7 @@
         <v>391</v>
       </c>
       <c r="D144" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="E144">
         <v>26</v>
@@ -5159,7 +5212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5170,7 +5223,7 @@
         <v>392</v>
       </c>
       <c r="D145" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="E145">
         <v>30</v>
@@ -5179,7 +5232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5199,7 +5252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5210,7 +5263,7 @@
         <v>394</v>
       </c>
       <c r="D147" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="E147">
         <v>11</v>
@@ -5219,7 +5272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5239,7 +5292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5259,7 +5312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5270,7 +5323,7 @@
         <v>397</v>
       </c>
       <c r="D150" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="E150">
         <v>12</v>
@@ -5279,7 +5332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5290,7 +5343,7 @@
         <v>398</v>
       </c>
       <c r="D151" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="E151">
         <v>18</v>
@@ -5299,7 +5352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5310,7 +5363,7 @@
         <v>399</v>
       </c>
       <c r="D152" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="E152">
         <v>16</v>
@@ -5319,7 +5372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5339,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5359,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5370,7 +5423,7 @@
         <v>402</v>
       </c>
       <c r="D155" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E155">
         <v>22</v>
@@ -5379,7 +5432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5399,7 +5452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5419,7 +5472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5439,7 +5492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5450,7 +5503,7 @@
         <v>406</v>
       </c>
       <c r="D159" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="E159">
         <v>11</v>
@@ -5459,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5470,7 +5523,7 @@
         <v>407</v>
       </c>
       <c r="D160" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E160">
         <v>17</v>
@@ -5479,7 +5532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5490,7 +5543,7 @@
         <v>408</v>
       </c>
       <c r="D161" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E161">
         <v>15</v>
@@ -5499,7 +5552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5510,7 +5563,7 @@
         <v>409</v>
       </c>
       <c r="D162" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E162">
         <v>29</v>
@@ -5519,7 +5572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5530,7 +5583,7 @@
         <v>410</v>
       </c>
       <c r="D163" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E163">
         <v>13</v>
@@ -5539,7 +5592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5550,7 +5603,7 @@
         <v>411</v>
       </c>
       <c r="D164" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E164">
         <v>25</v>
@@ -5559,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5570,7 +5623,7 @@
         <v>412</v>
       </c>
       <c r="D165" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="E165">
         <v>13</v>
@@ -5579,7 +5632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5590,7 +5643,7 @@
         <v>413</v>
       </c>
       <c r="D166" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="E166">
         <v>7</v>
@@ -5599,7 +5652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5610,7 +5663,7 @@
         <v>414</v>
       </c>
       <c r="D167" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E167">
         <v>22</v>
@@ -5619,7 +5672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5630,7 +5683,7 @@
         <v>415</v>
       </c>
       <c r="D168" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E168">
         <v>18</v>
@@ -5639,7 +5692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5650,7 +5703,7 @@
         <v>416</v>
       </c>
       <c r="D169" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E169">
         <v>18</v>
@@ -5659,7 +5712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5670,7 +5723,7 @@
         <v>417</v>
       </c>
       <c r="D170" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E170">
         <v>16</v>
@@ -5679,7 +5732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5690,7 +5743,7 @@
         <v>418</v>
       </c>
       <c r="D171" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E171">
         <v>17</v>
@@ -5699,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5710,7 +5763,7 @@
         <v>419</v>
       </c>
       <c r="D172" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E172">
         <v>10</v>
@@ -5719,7 +5772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5730,7 +5783,7 @@
         <v>420</v>
       </c>
       <c r="D173" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E173">
         <v>22</v>
@@ -5739,7 +5792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5750,7 +5803,7 @@
         <v>421</v>
       </c>
       <c r="D174" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E174">
         <v>20</v>
@@ -5759,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5770,7 +5823,7 @@
         <v>422</v>
       </c>
       <c r="D175" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E175">
         <v>24</v>
@@ -5779,7 +5832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5790,7 +5843,7 @@
         <v>423</v>
       </c>
       <c r="D176" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E176">
         <v>21</v>
@@ -5799,7 +5852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5810,7 +5863,7 @@
         <v>424</v>
       </c>
       <c r="D177" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E177">
         <v>21</v>
@@ -5819,7 +5872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5839,7 +5892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5859,7 +5912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5870,7 +5923,7 @@
         <v>427</v>
       </c>
       <c r="D180" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="E180">
         <v>29</v>
@@ -5879,7 +5932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5890,7 +5943,7 @@
         <v>428</v>
       </c>
       <c r="D181" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="E181">
         <v>35</v>
@@ -5899,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5919,7 +5972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5930,7 +5983,7 @@
         <v>430</v>
       </c>
       <c r="D183" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="E183">
         <v>20</v>
@@ -5939,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5950,7 +6003,7 @@
         <v>431</v>
       </c>
       <c r="D184" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="E184">
         <v>30</v>
@@ -5959,7 +6012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5970,7 +6023,7 @@
         <v>432</v>
       </c>
       <c r="D185" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E185">
         <v>12</v>
@@ -5979,7 +6032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5990,7 +6043,7 @@
         <v>433</v>
       </c>
       <c r="D186" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="E186">
         <v>51</v>
@@ -5999,7 +6052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6010,7 +6063,7 @@
         <v>434</v>
       </c>
       <c r="D187" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="E187">
         <v>17</v>
@@ -6019,7 +6072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6030,7 +6083,7 @@
         <v>435</v>
       </c>
       <c r="D188" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="E188">
         <v>23</v>
@@ -6039,7 +6092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6050,7 +6103,7 @@
         <v>436</v>
       </c>
       <c r="D189" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="E189">
         <v>5</v>
@@ -6059,7 +6112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6070,7 +6123,7 @@
         <v>437</v>
       </c>
       <c r="D190" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E190">
         <v>21</v>
@@ -6079,7 +6132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6099,7 +6152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6119,7 +6172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6139,7 +6192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6150,7 +6203,7 @@
         <v>441</v>
       </c>
       <c r="D194" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="E194">
         <v>11</v>
@@ -6159,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6170,7 +6223,7 @@
         <v>442</v>
       </c>
       <c r="D195" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E195">
         <v>14</v>
@@ -6179,7 +6232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6199,7 +6252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6210,7 +6263,7 @@
         <v>444</v>
       </c>
       <c r="D197" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E197">
         <v>28</v>
@@ -6219,7 +6272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6230,7 +6283,7 @@
         <v>445</v>
       </c>
       <c r="D198" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="E198">
         <v>21</v>
@@ -6239,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6250,7 +6303,7 @@
         <v>446</v>
       </c>
       <c r="D199" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E199">
         <v>24</v>
@@ -6259,7 +6312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6270,7 +6323,7 @@
         <v>447</v>
       </c>
       <c r="D200" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E200">
         <v>27</v>
@@ -6279,7 +6332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6290,7 +6343,7 @@
         <v>448</v>
       </c>
       <c r="D201" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E201">
         <v>42</v>
@@ -6299,7 +6352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6310,7 +6363,7 @@
         <v>449</v>
       </c>
       <c r="D202" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="E202">
         <v>18</v>
@@ -6319,7 +6372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6330,7 +6383,7 @@
         <v>450</v>
       </c>
       <c r="D203" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E203">
         <v>14</v>
@@ -6339,7 +6392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6350,7 +6403,7 @@
         <v>451</v>
       </c>
       <c r="D204" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E204">
         <v>28</v>
@@ -6359,7 +6412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6370,7 +6423,7 @@
         <v>452</v>
       </c>
       <c r="D205" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="E205">
         <v>26</v>
@@ -6379,7 +6432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6390,7 +6443,7 @@
         <v>453</v>
       </c>
       <c r="D206" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E206">
         <v>30</v>
@@ -6399,7 +6452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6410,7 +6463,7 @@
         <v>454</v>
       </c>
       <c r="D207" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="E207">
         <v>24</v>
@@ -6419,7 +6472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6430,7 +6483,7 @@
         <v>455</v>
       </c>
       <c r="D208" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E208">
         <v>22</v>
@@ -6439,7 +6492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6450,7 +6503,7 @@
         <v>456</v>
       </c>
       <c r="D209" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="E209">
         <v>22</v>
@@ -6459,7 +6512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -6470,7 +6523,7 @@
         <v>457</v>
       </c>
       <c r="D210" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="E210">
         <v>19</v>
@@ -6479,7 +6532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -6490,7 +6543,7 @@
         <v>458</v>
       </c>
       <c r="D211" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="E211">
         <v>24</v>
@@ -6499,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -6510,7 +6563,7 @@
         <v>459</v>
       </c>
       <c r="D212" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="E212">
         <v>20</v>
@@ -6519,7 +6572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -6539,7 +6592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -6559,7 +6612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -6570,7 +6623,7 @@
         <v>462</v>
       </c>
       <c r="D215" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="E215">
         <v>30</v>
@@ -6579,7 +6632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:6">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -6599,7 +6652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -6619,7 +6672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:6">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -6639,7 +6692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:6">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -6650,7 +6703,7 @@
         <v>466</v>
       </c>
       <c r="D219" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E219">
         <v>18</v>
@@ -6659,7 +6712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -6679,7 +6732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -6699,7 +6752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -6719,7 +6772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -6739,7 +6792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -6759,7 +6812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -6779,7 +6832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -6790,7 +6843,7 @@
         <v>473</v>
       </c>
       <c r="D226" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="E226">
         <v>15</v>
@@ -6799,7 +6852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:6">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -6810,7 +6863,7 @@
         <v>474</v>
       </c>
       <c r="D227" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="E227">
         <v>35</v>
@@ -6819,7 +6872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -6830,7 +6883,7 @@
         <v>475</v>
       </c>
       <c r="D228" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E228">
         <v>28</v>
@@ -6839,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:6">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -6859,7 +6912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -6879,7 +6932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:6">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -6890,7 +6943,7 @@
         <v>478</v>
       </c>
       <c r="D231" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E231">
         <v>18</v>
@@ -6899,7 +6952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:6">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -6919,7 +6972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:6">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -6939,7 +6992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -6950,7 +7003,7 @@
         <v>481</v>
       </c>
       <c r="D234" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E234">
         <v>33</v>
@@ -6959,7 +7012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:6">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -6970,7 +7023,7 @@
         <v>482</v>
       </c>
       <c r="D235" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E235">
         <v>16</v>
@@ -6979,7 +7032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:6">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -6990,7 +7043,7 @@
         <v>483</v>
       </c>
       <c r="D236" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E236">
         <v>19</v>
@@ -6999,7 +7052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -7019,7 +7072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:6">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -7030,7 +7083,7 @@
         <v>485</v>
       </c>
       <c r="D238" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="E238">
         <v>23</v>
@@ -7039,7 +7092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:6">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -7059,7 +7112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:6">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
@@ -7079,7 +7132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -7090,7 +7143,7 @@
         <v>488</v>
       </c>
       <c r="D241" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E241">
         <v>4</v>
@@ -7099,7 +7152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>247</v>
       </c>
@@ -7107,7 +7160,7 @@
         <v>489</v>
       </c>
       <c r="D242" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E242">
         <v>13</v>
@@ -7119,7 +7172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>248</v>
       </c>
@@ -7127,7 +7180,7 @@
         <v>490</v>
       </c>
       <c r="D243" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="E243">
         <v>17</v>

</xml_diff>

<commit_message>
theme table rounding order fixed
</commit_message>
<xml_diff>
--- a/DataInput/Updated_Yan-Zheng-Compustat-Vars.xlsx
+++ b/DataInput/Updated_Yan-Zheng-Compustat-Vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Risk-vs-ac\flex-mining\DataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20B8FFC-C1F5-45FD-B844-0582028E367D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39FDAFF-6705-4563-8EBA-4D1ABA1A98CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="-120" windowWidth="26775" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1729,9 +1729,6 @@
     <t>Op income after deprec</t>
   </si>
   <si>
-    <t>PPE (gross)</t>
-  </si>
-  <si>
     <t>PPE buildings net</t>
   </si>
   <si>
@@ -1928,6 +1925,9 @@
   </si>
   <si>
     <t>Income bef extraord common</t>
+  </si>
+  <si>
+    <t>PPE gross</t>
   </si>
 </sst>
 </file>
@@ -2311,8 +2311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2349,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E13">
         <v>32</v>
@@ -2603,7 +2603,7 @@
         <v>261</v>
       </c>
       <c r="D14" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E14">
         <v>31</v>
@@ -2663,7 +2663,7 @@
         <v>264</v>
       </c>
       <c r="D17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E17">
         <v>19</v>
@@ -2983,7 +2983,7 @@
         <v>280</v>
       </c>
       <c r="D33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E33">
         <v>39</v>
@@ -4503,7 +4503,7 @@
         <v>356</v>
       </c>
       <c r="D109" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E109">
         <v>36</v>
@@ -4523,7 +4523,7 @@
         <v>357</v>
       </c>
       <c r="D110" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E110">
         <v>23</v>
@@ -5503,7 +5503,7 @@
         <v>406</v>
       </c>
       <c r="D159" t="s">
-        <v>569</v>
+        <v>635</v>
       </c>
       <c r="E159">
         <v>11</v>
@@ -5523,7 +5523,7 @@
         <v>407</v>
       </c>
       <c r="D160" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E160">
         <v>17</v>
@@ -5543,7 +5543,7 @@
         <v>408</v>
       </c>
       <c r="D161" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E161">
         <v>15</v>
@@ -5563,7 +5563,7 @@
         <v>409</v>
       </c>
       <c r="D162" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E162">
         <v>29</v>
@@ -5583,7 +5583,7 @@
         <v>410</v>
       </c>
       <c r="D163" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E163">
         <v>13</v>
@@ -5603,7 +5603,7 @@
         <v>411</v>
       </c>
       <c r="D164" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E164">
         <v>25</v>
@@ -5623,7 +5623,7 @@
         <v>412</v>
       </c>
       <c r="D165" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E165">
         <v>13</v>
@@ -5643,7 +5643,7 @@
         <v>413</v>
       </c>
       <c r="D166" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E166">
         <v>7</v>
@@ -5663,7 +5663,7 @@
         <v>414</v>
       </c>
       <c r="D167" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E167">
         <v>22</v>
@@ -5683,7 +5683,7 @@
         <v>415</v>
       </c>
       <c r="D168" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E168">
         <v>18</v>
@@ -5703,7 +5703,7 @@
         <v>416</v>
       </c>
       <c r="D169" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E169">
         <v>18</v>
@@ -5723,7 +5723,7 @@
         <v>417</v>
       </c>
       <c r="D170" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E170">
         <v>16</v>
@@ -5743,7 +5743,7 @@
         <v>418</v>
       </c>
       <c r="D171" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E171">
         <v>17</v>
@@ -5763,7 +5763,7 @@
         <v>419</v>
       </c>
       <c r="D172" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E172">
         <v>10</v>
@@ -5783,7 +5783,7 @@
         <v>420</v>
       </c>
       <c r="D173" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E173">
         <v>22</v>
@@ -5803,7 +5803,7 @@
         <v>421</v>
       </c>
       <c r="D174" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E174">
         <v>20</v>
@@ -5823,7 +5823,7 @@
         <v>422</v>
       </c>
       <c r="D175" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E175">
         <v>24</v>
@@ -5843,7 +5843,7 @@
         <v>423</v>
       </c>
       <c r="D176" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E176">
         <v>21</v>
@@ -5863,7 +5863,7 @@
         <v>424</v>
       </c>
       <c r="D177" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E177">
         <v>21</v>
@@ -5923,7 +5923,7 @@
         <v>427</v>
       </c>
       <c r="D180" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E180">
         <v>29</v>
@@ -5943,7 +5943,7 @@
         <v>428</v>
       </c>
       <c r="D181" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E181">
         <v>35</v>
@@ -5983,7 +5983,7 @@
         <v>430</v>
       </c>
       <c r="D183" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E183">
         <v>20</v>
@@ -6003,7 +6003,7 @@
         <v>431</v>
       </c>
       <c r="D184" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E184">
         <v>30</v>
@@ -6023,7 +6023,7 @@
         <v>432</v>
       </c>
       <c r="D185" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E185">
         <v>12</v>
@@ -6043,7 +6043,7 @@
         <v>433</v>
       </c>
       <c r="D186" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E186">
         <v>51</v>
@@ -6063,7 +6063,7 @@
         <v>434</v>
       </c>
       <c r="D187" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E187">
         <v>17</v>
@@ -6083,7 +6083,7 @@
         <v>435</v>
       </c>
       <c r="D188" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E188">
         <v>23</v>
@@ -6103,7 +6103,7 @@
         <v>436</v>
       </c>
       <c r="D189" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E189">
         <v>5</v>
@@ -6123,7 +6123,7 @@
         <v>437</v>
       </c>
       <c r="D190" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E190">
         <v>21</v>
@@ -6203,7 +6203,7 @@
         <v>441</v>
       </c>
       <c r="D194" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E194">
         <v>11</v>
@@ -6223,7 +6223,7 @@
         <v>442</v>
       </c>
       <c r="D195" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E195">
         <v>14</v>
@@ -6263,7 +6263,7 @@
         <v>444</v>
       </c>
       <c r="D197" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E197">
         <v>28</v>
@@ -6283,7 +6283,7 @@
         <v>445</v>
       </c>
       <c r="D198" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E198">
         <v>21</v>
@@ -6303,7 +6303,7 @@
         <v>446</v>
       </c>
       <c r="D199" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E199">
         <v>24</v>
@@ -6323,7 +6323,7 @@
         <v>447</v>
       </c>
       <c r="D200" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E200">
         <v>27</v>
@@ -6343,7 +6343,7 @@
         <v>448</v>
       </c>
       <c r="D201" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E201">
         <v>42</v>
@@ -6363,7 +6363,7 @@
         <v>449</v>
       </c>
       <c r="D202" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E202">
         <v>18</v>
@@ -6383,7 +6383,7 @@
         <v>450</v>
       </c>
       <c r="D203" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E203">
         <v>14</v>
@@ -6403,7 +6403,7 @@
         <v>451</v>
       </c>
       <c r="D204" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E204">
         <v>28</v>
@@ -6423,7 +6423,7 @@
         <v>452</v>
       </c>
       <c r="D205" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E205">
         <v>26</v>
@@ -6443,7 +6443,7 @@
         <v>453</v>
       </c>
       <c r="D206" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E206">
         <v>30</v>
@@ -6463,7 +6463,7 @@
         <v>454</v>
       </c>
       <c r="D207" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E207">
         <v>24</v>
@@ -6483,7 +6483,7 @@
         <v>455</v>
       </c>
       <c r="D208" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E208">
         <v>22</v>
@@ -6503,7 +6503,7 @@
         <v>456</v>
       </c>
       <c r="D209" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E209">
         <v>22</v>
@@ -6523,7 +6523,7 @@
         <v>457</v>
       </c>
       <c r="D210" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E210">
         <v>19</v>
@@ -6543,7 +6543,7 @@
         <v>458</v>
       </c>
       <c r="D211" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E211">
         <v>24</v>
@@ -6563,7 +6563,7 @@
         <v>459</v>
       </c>
       <c r="D212" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E212">
         <v>20</v>
@@ -6623,7 +6623,7 @@
         <v>462</v>
       </c>
       <c r="D215" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E215">
         <v>30</v>
@@ -6703,7 +6703,7 @@
         <v>466</v>
       </c>
       <c r="D219" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E219">
         <v>18</v>
@@ -6843,7 +6843,7 @@
         <v>473</v>
       </c>
       <c r="D226" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E226">
         <v>15</v>
@@ -6863,7 +6863,7 @@
         <v>474</v>
       </c>
       <c r="D227" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E227">
         <v>35</v>
@@ -6883,7 +6883,7 @@
         <v>475</v>
       </c>
       <c r="D228" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E228">
         <v>28</v>
@@ -6943,7 +6943,7 @@
         <v>478</v>
       </c>
       <c r="D231" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E231">
         <v>18</v>
@@ -7003,7 +7003,7 @@
         <v>481</v>
       </c>
       <c r="D234" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E234">
         <v>33</v>
@@ -7023,7 +7023,7 @@
         <v>482</v>
       </c>
       <c r="D235" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E235">
         <v>16</v>
@@ -7043,7 +7043,7 @@
         <v>483</v>
       </c>
       <c r="D236" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E236">
         <v>19</v>
@@ -7083,7 +7083,7 @@
         <v>485</v>
       </c>
       <c r="D238" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E238">
         <v>23</v>
@@ -7143,7 +7143,7 @@
         <v>488</v>
       </c>
       <c r="D241" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E241">
         <v>4</v>
@@ -7160,7 +7160,7 @@
         <v>489</v>
       </c>
       <c r="D242" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E242">
         <v>13</v>
@@ -7180,7 +7180,7 @@
         <v>490</v>
       </c>
       <c r="D243" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E243">
         <v>17</v>

</xml_diff>